<commit_message>
Save local Search to excel
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jobList.xlsx
+++ b/src/test/resources/data/jobList.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="217">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -532,6 +532,153 @@
   </si>
   <si>
     <t>https://uk.indeed.com/company/Zoonou/jobs/QA-Test-Analyst-1722784dfeca123a?fccid=e845c5dd58d11526&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>SDET - Software Development Engineer in Test, Cloud (Remote)</t>
+  </si>
+  <si>
+    <t>Senior SDET</t>
+  </si>
+  <si>
+    <t>Junior SDET / Test Engineer (Python Automation)</t>
+  </si>
+  <si>
+    <t>SDET</t>
+  </si>
+  <si>
+    <t>Software Development Engineer in Test (SDET)</t>
+  </si>
+  <si>
+    <t>Senior Consultant - Software Development Engineer in Test (S...</t>
+  </si>
+  <si>
+    <t>Software Engineering in Test SDET</t>
+  </si>
+  <si>
+    <t>Snr SDET</t>
+  </si>
+  <si>
+    <t>Automation Test Engineer / SDET (Java)</t>
+  </si>
+  <si>
+    <t>Software Development Engineer in Test - Android (Remote, GBR...</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/rc/clk?jk=2316c31070f8ab52&amp;fccid=c44218d8c2035787&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/rc/clk?jk=24608845c54829f9&amp;fccid=64e4cdd7435d8c42&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/rc/clk?jk=b258128b3092eb08&amp;fccid=447163ca34a4b3d8&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/rc/clk?jk=f6b779cf20637696&amp;fccid=36e692c6802aae6c&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/rc/clk?jk=89a02e36c7c8699a&amp;fccid=04f36097f3ddf22e&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/rc/clk?jk=abbf0a62614c053f&amp;fccid=e3b893882ce68e4d&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/rc/clk?jk=36c06d78b4183142&amp;fccid=9e215d88a6b33622&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/rc/clk?jk=ec4d09e700092c5b&amp;fccid=1d6acce86770faa4&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/rc/clk?jk=d293545f2078cefd&amp;fccid=bfd62d072447f458&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/company/Qumu/jobs/Snr-Sdet-ba16e3dfbdb2d38b?fccid=77a8dc935ac1a44a&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/rc/clk?jk=c5be219e12ad9004&amp;fccid=c44218d8c2035787&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/rc/clk?jk=bedea54b9ae2530e&amp;fccid=64e4cdd7435d8c42&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/rc/clk?jk=e65125fb4a30f046&amp;fccid=0288b34a02030660&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>SDET - Software Development engineer in Test (Remote, GBR)</t>
+  </si>
+  <si>
+    <t>Software Engineer - SDET</t>
+  </si>
+  <si>
+    <t>Software Developer in Test CONTRACT</t>
+  </si>
+  <si>
+    <t>Senior QA Engineer C# SDET (Remote) £50k</t>
+  </si>
+  <si>
+    <t>Lead Java (SDET) Software Developer In Test</t>
+  </si>
+  <si>
+    <t>Contract python test developer</t>
+  </si>
+  <si>
+    <t>C# Automation Tester</t>
+  </si>
+  <si>
+    <t>Lead Automation Tester | Remote | Up to £70,000</t>
+  </si>
+  <si>
+    <t>Python Test Automation Engineer</t>
+  </si>
+  <si>
+    <t>Senior SDET / Test Engineer (Python Automation)</t>
+  </si>
+  <si>
+    <t>Full stack AWS Software Engineer</t>
+  </si>
+  <si>
+    <t>Lead JavaScript / React (SDET) Software Developer</t>
+  </si>
+  <si>
+    <t>Software Development Engineer in Test - iOS (Remote, GBR)</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/rc/clk?jk=9db39558b28f92e1&amp;fccid=64e4cdd7435d8c42&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/rc/clk?jk=82db1474bc87c15e&amp;fccid=9526cf37acc8babe&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/rc/clk?jk=c04a5ccae68f8e6b&amp;fccid=8f35589a37e69470&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/rc/clk?jk=2f3f5beb9b30196c&amp;fccid=dd616958bd9ddc12&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/rc/clk?jk=e1b8747527ff5ea8&amp;fccid=d6830df36521c563&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/rc/clk?jk=705320533dc92838&amp;fccid=8f35589a37e69470&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/rc/clk?jk=68ee8a1ac1c3694e&amp;fccid=a77d4b706742e9cb&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/rc/clk?jk=5d901ccb1ab672e1&amp;fccid=77087bd1709a8148&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/rc/clk?jk=7cf17be453a87cec&amp;fccid=8f35589a37e69470&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/rc/clk?jk=f0eda2f03e9d44d0&amp;fccid=36e692c6802aae6c&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/rc/clk?jk=c4d3348ac900b88e&amp;fccid=d50c573274bf1c1f&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/rc/clk?jk=c73c463081e061a5&amp;fccid=d6830df36521c563&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/rc/clk?jk=4db609371d728498&amp;fccid=64e4cdd7435d8c42&amp;vjs=3</t>
   </si>
 </sst>
 </file>
@@ -654,106 +801,106 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>103</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>17</v>
+        <v>168</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>104</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>21</v>
+        <v>169</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>105</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>31</v>
+        <v>170</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>106</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>44</v>
+        <v>171</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>107</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>25</v>
+        <v>172</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>108</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>24</v>
+        <v>173</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>109</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>110</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>42</v>
+        <v>174</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>111</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>112</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>20</v>
+        <v>176</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>113</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>43</v>
+        <v>177</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>114</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>115</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -794,106 +941,106 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>31</v>
+        <v>191</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>116</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>66</v>
+        <v>192</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>117</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>20</v>
+        <v>193</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>118</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>68</v>
+        <v>194</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>119</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>40</v>
+        <v>195</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>120</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>35</v>
+        <v>196</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>121</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>34</v>
+        <v>197</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>122</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>20</v>
+        <v>198</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>123</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>64</v>
+        <v>199</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>124</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>69</v>
+        <v>200</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>125</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>19</v>
+        <v>201</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>126</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>70</v>
+        <v>202</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>127</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>46</v>
+        <v>203</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>128</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Serach on 16 Sept
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jobList.xlsx
+++ b/src/test/resources/data/jobList.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="219">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -679,6 +679,12 @@
   </si>
   <si>
     <t>https://uk.indeed.com/rc/clk?jk=4db609371d728498&amp;fccid=64e4cdd7435d8c42&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>Software Engineer in Test (SDET)</t>
+  </si>
+  <si>
+    <t>https://uk.indeed.com/rc/clk?jk=fd9e8860b3959cc4&amp;fccid=c659788ec6cc356e&amp;vjs=3</t>
   </si>
 </sst>
 </file>
@@ -801,18 +807,18 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>61</v>
+        <v>196</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>178</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>168</v>
+        <v>217</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>179</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>